<commit_message>
Added original huang experiment folder
</commit_message>
<xml_diff>
--- a/Condition1.xlsx
+++ b/Condition1.xlsx
@@ -1,29 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20338"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4171D15E-A685-3A4A-B2CE-DD23ED2AB1C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6348D0E-0288-45B7-96D8-ACF027986428}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8532" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
@@ -42,22 +29,22 @@
     <t>SoundName</t>
   </si>
   <si>
-    <t>Condition/CS+1.BMP</t>
+    <t>Condition\black.PNG</t>
   </si>
   <si>
-    <t>Condition/black.PNG</t>
+    <t>Sound\silent.wav</t>
   </si>
   <si>
-    <t>Sound/silent.wav</t>
+    <t>Sound\scream1.wav</t>
   </si>
   <si>
-    <t>Condition/UCS1.BMP</t>
+    <t>Condition\CS+1.BMP</t>
   </si>
   <si>
-    <t>Sound/scream1.wav</t>
+    <t>Condition\CS-1.BMP</t>
   </si>
   <si>
-    <t>Condition/CS-1.BMP</t>
+    <t>Condition\UCS1.BMP</t>
   </si>
 </sst>
 </file>
@@ -113,7 +100,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -129,7 +116,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -451,19 +438,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" customWidth="1"/>
-    <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="3" width="19.83203125" customWidth="1"/>
-    <col min="4" max="4" width="12.5"/>
+    <col min="1" max="1" width="20.77734375" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" customWidth="1"/>
+    <col min="3" max="3" width="19.77734375" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -477,421 +464,421 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2">
         <v>-0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="2">
         <v>-0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" s="2">
         <v>-0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D5" s="2">
         <v>0.9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D6" s="2">
         <v>0.9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D7" s="2">
         <v>0.9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D8" s="2">
         <v>0.9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D9" s="2">
         <v>0.9</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D10" s="2">
         <v>0.9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D11" s="2">
         <v>0.9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D12" s="2">
         <v>0.9</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D13" s="2">
         <v>0.9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D14" s="2">
         <v>0.9</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D15" s="2">
         <v>0.9</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D16" s="2">
         <v>0.9</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D17" s="2">
         <v>0.4</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D18" s="2">
         <v>0.4</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D19" s="2">
         <v>0.4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D20" s="2">
         <v>0.4</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D21" s="2">
         <v>0.4</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D22" s="2">
         <v>0.4</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D23" s="2">
         <v>0.4</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D24" s="2">
         <v>0.4</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D25" s="2">
         <v>0.4</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D26" s="2">
         <v>0.4</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D27" s="2">
         <v>0.4</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D28" s="2">
         <v>0.4</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D29" s="2">
         <v>0.4</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D30" s="2">
         <v>0.4</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D31" s="2">
         <v>0.4</v>
@@ -909,15 +896,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DCC15C826F9CD04C984C1E59D79D0BF3" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4323ffbe69f4456b442358682c62cfba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="64b0b0ad-49a7-4b34-8eba-9a240439451d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="94ec3c4b7e8ae219eb184f3ca94c286d" ns2:_="">
     <xsd:import namespace="64b0b0ad-49a7-4b34-8eba-9a240439451d"/>
@@ -1101,6 +1079,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F795CB29-6365-4DA8-8C2F-885C5D31C81A}">
   <ds:schemaRefs>
@@ -1111,14 +1098,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4BCAEFB8-08FC-4F45-B367-68A06CA5E545}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{899E66D0-C9AE-42BF-A4B6-2A0DE66F65C9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1134,4 +1113,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4BCAEFB8-08FC-4F45-B367-68A06CA5E545}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Reduced to 3 stim, added gray circles
</commit_message>
<xml_diff>
--- a/Condition1.xlsx
+++ b/Condition1.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11211"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4171D15E-A685-3A4A-B2CE-DD23ED2AB1C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6285B7B2-83D9-C54A-BBCE-039ED38AAD9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19200" yWindow="-2760" windowWidth="19200" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="13">
   <si>
     <t>TrgCol</t>
   </si>
@@ -42,22 +42,31 @@
     <t>SoundName</t>
   </si>
   <si>
-    <t>Condition/CS+1.BMP</t>
-  </si>
-  <si>
-    <t>Condition/black.PNG</t>
-  </si>
-  <si>
     <t>Sound/silent.wav</t>
-  </si>
-  <si>
-    <t>Condition/UCS1.BMP</t>
   </si>
   <si>
     <t>Sound/scream1.wav</t>
   </si>
   <si>
-    <t>Condition/CS-1.BMP</t>
+    <t>Stimuli/CS+1.BMP</t>
+  </si>
+  <si>
+    <t>Stimuli/black.PNG</t>
+  </si>
+  <si>
+    <t>Stimuli/UCS1.BMP</t>
+  </si>
+  <si>
+    <t>Stimuli/CS+3.BMP</t>
+  </si>
+  <si>
+    <t>Stimuli/CS+4.BMP</t>
+  </si>
+  <si>
+    <t>Stimuli/UCS4.BMP</t>
+  </si>
+  <si>
+    <t>Sound/laugh1.wav</t>
   </si>
 </sst>
 </file>
@@ -86,12 +95,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -106,11 +121,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -129,7 +147,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -449,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -477,213 +495,213 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="5">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="5">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="5">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2">
-        <v>-0.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="D5" s="5">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="2">
-        <v>-0.1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="D6" s="5">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="2">
-        <v>-0.1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="D7" s="5">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="2">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="C8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="2">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="C9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="2">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="C10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="2">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="C11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="2">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="C12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="2">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="C13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="2">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="C14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="5">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="2">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="C15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="5">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="2">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="2">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="2">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="2">
+      <c r="C16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="5">
         <v>0.9</v>
       </c>
     </row>
@@ -692,10 +710,10 @@
         <v>9</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D17" s="2">
         <v>0.4</v>
@@ -706,10 +724,10 @@
         <v>9</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D18" s="2">
         <v>0.4</v>
@@ -720,10 +738,10 @@
         <v>9</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D19" s="2">
         <v>0.4</v>
@@ -734,10 +752,10 @@
         <v>9</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D20" s="2">
         <v>0.4</v>
@@ -748,10 +766,10 @@
         <v>9</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D21" s="2">
         <v>0.4</v>
@@ -762,10 +780,10 @@
         <v>9</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D22" s="2">
         <v>0.4</v>
@@ -776,10 +794,10 @@
         <v>9</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D23" s="2">
         <v>0.4</v>
@@ -790,10 +808,10 @@
         <v>9</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D24" s="2">
         <v>0.4</v>
@@ -804,10 +822,10 @@
         <v>9</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D25" s="2">
         <v>0.4</v>
@@ -818,10 +836,10 @@
         <v>9</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D26" s="2">
         <v>0.4</v>
@@ -832,10 +850,10 @@
         <v>9</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D27" s="2">
         <v>0.4</v>
@@ -846,10 +864,10 @@
         <v>9</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D28" s="2">
         <v>0.4</v>
@@ -860,10 +878,10 @@
         <v>9</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D29" s="2">
         <v>0.4</v>
@@ -874,27 +892,237 @@
         <v>9</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D30" s="2">
         <v>0.4</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="2">
-        <v>0.4</v>
+        <v>4</v>
+      </c>
+      <c r="D31" s="6">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="5">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="5">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="5">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" s="5">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" s="5">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" s="5">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38" s="5">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39" s="5">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" s="5">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D41" s="5">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A42" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D42" s="5">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A43" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D43" s="5">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A44" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D44" s="5">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D45" s="5">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D46" s="5">
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>
@@ -903,21 +1131,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DCC15C826F9CD04C984C1E59D79D0BF3" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4323ffbe69f4456b442358682c62cfba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="64b0b0ad-49a7-4b34-8eba-9a240439451d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="94ec3c4b7e8ae219eb184f3ca94c286d" ns2:_="">
     <xsd:import namespace="64b0b0ad-49a7-4b34-8eba-9a240439451d"/>
@@ -1101,24 +1314,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F795CB29-6365-4DA8-8C2F-885C5D31C81A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4BCAEFB8-08FC-4F45-B367-68A06CA5E545}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{899E66D0-C9AE-42BF-A4B6-2A0DE66F65C9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1134,4 +1345,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F795CB29-6365-4DA8-8C2F-885C5D31C81A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4BCAEFB8-08FC-4F45-B367-68A06CA5E545}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>